<commit_message>
samenvatting van data toegevoegd
</commit_message>
<xml_diff>
--- a/bachproef/BP_test_values_summary.xlsx
+++ b/bachproef/BP_test_values_summary.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wannes\Documents\BP_WannesDT_SwiftUI\bachproef\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A8A01-68B6-4A8D-91DC-27AB73E750EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D962830E-DA37-4D62-936A-4B0188E2DE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7290" yWindow="4170" windowWidth="15180" windowHeight="14400" xr2:uid="{60AB8C76-5F9D-41FD-8518-CA5CB2C3E509}"/>
+    <workbookView xWindow="-7530" yWindow="4755" windowWidth="15180" windowHeight="14400" activeTab="2" xr2:uid="{60AB8C76-5F9D-41FD-8518-CA5CB2C3E509}"/>
   </bookViews>
   <sheets>
     <sheet name="test2 subviews" sheetId="1" r:id="rId1"/>
+    <sheet name="test3 lazy" sheetId="2" r:id="rId2"/>
+    <sheet name="test4 non-lazy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="96">
   <si>
     <t>Binding</t>
   </si>
@@ -186,13 +188,151 @@
   </si>
   <si>
     <t>653.23 Mc</t>
+  </si>
+  <si>
+    <t>936,85 Mc</t>
+  </si>
+  <si>
+    <t>666 ms</t>
+  </si>
+  <si>
+    <t>269,46 µs</t>
+  </si>
+  <si>
+    <t>1,93 ms</t>
+  </si>
+  <si>
+    <t>2,30 ms</t>
+  </si>
+  <si>
+    <t>26,95 µs</t>
+  </si>
+  <si>
+    <t>21,48 µs</t>
+  </si>
+  <si>
+    <t>429,49 Mc</t>
+  </si>
+  <si>
+    <t>609 ms</t>
+  </si>
+  <si>
+    <t>1,85 ms</t>
+  </si>
+  <si>
+    <t>N.VT</t>
+  </si>
+  <si>
+    <t>20,50 µs</t>
+  </si>
+  <si>
+    <t>463,30 Mc</t>
+  </si>
+  <si>
+    <t>927 ms</t>
+  </si>
+  <si>
+    <t>40,25 µs</t>
+  </si>
+  <si>
+    <t>20,97 µs</t>
+  </si>
+  <si>
+    <t>2,08 ms</t>
+  </si>
+  <si>
+    <t>2,12 ms</t>
+  </si>
+  <si>
+    <t>862,21 Mc</t>
+  </si>
+  <si>
+    <t>515 ms</t>
+  </si>
+  <si>
+    <t>2,1 ms</t>
+  </si>
+  <si>
+    <t>23,33 µs</t>
+  </si>
+  <si>
+    <t>12,93 Gc</t>
+  </si>
+  <si>
+    <t>Gc = GigaCycles</t>
+  </si>
+  <si>
+    <t>6,02 s</t>
+  </si>
+  <si>
+    <t>30,15 ms</t>
+  </si>
+  <si>
+    <t>209,96 µs</t>
+  </si>
+  <si>
+    <t>30,36 ms</t>
+  </si>
+  <si>
+    <t>6,87  µs</t>
+  </si>
+  <si>
+    <t>6,84  µs</t>
+  </si>
+  <si>
+    <t>12,10 Gc</t>
+  </si>
+  <si>
+    <t>4,77 s</t>
+  </si>
+  <si>
+    <t>24,49 ms</t>
+  </si>
+  <si>
+    <t>5,55 µs</t>
+  </si>
+  <si>
+    <t>12,19 Gc</t>
+  </si>
+  <si>
+    <t>4,8 s</t>
+  </si>
+  <si>
+    <t>23,24 ms</t>
+  </si>
+  <si>
+    <t>5,27 µs</t>
+  </si>
+  <si>
+    <t>12,04 Gc</t>
+  </si>
+  <si>
+    <t>4,81 s</t>
+  </si>
+  <si>
+    <t>24,33 ms</t>
+  </si>
+  <si>
+    <t>5,52 µs</t>
+  </si>
+  <si>
+    <t>Beste</t>
+  </si>
+  <si>
+    <t>Slechtste</t>
+  </si>
+  <si>
+    <t>beste</t>
+  </si>
+  <si>
+    <t>slechtste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,8 +363,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +380,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,17 +408,158 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -345,6 +644,206 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -359,14 +858,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98762B35-F5B4-4A66-829F-8C9732910B18}" name="Tabel3" displayName="Tabel3" ref="B4:F25" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98762B35-F5B4-4A66-829F-8C9732910B18}" name="Tabel3" displayName="Tabel3" ref="B4:F25" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="B4:F25" xr:uid="{98762B35-F5B4-4A66-829F-8C9732910B18}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{17186CD5-3871-4CF8-9282-BF72E8C1122C}" name="Description" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E122151B-C20D-493E-993E-F23AABB3D9C2}" name="Binding" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{71B98047-E9D6-4C40-A1A5-82DF558ABC9D}" name="Observable" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{70F1F426-807A-4A21-A9D8-60335B4EEF08}" name="EnvironmentObject" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0FA8658F-B54B-4B93-A47B-2612FAF06A72}" name="ObservableObject" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{17186CD5-3871-4CF8-9282-BF72E8C1122C}" name="Description" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{E122151B-C20D-493E-993E-F23AABB3D9C2}" name="Binding" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{71B98047-E9D6-4C40-A1A5-82DF558ABC9D}" name="Observable" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{70F1F426-807A-4A21-A9D8-60335B4EEF08}" name="EnvironmentObject" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{0FA8658F-B54B-4B93-A47B-2612FAF06A72}" name="ObservableObject" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D0BB9C06-469C-46FE-BB4D-C953A54DDCD0}" name="Tabel35" displayName="Tabel35" ref="H4:L25" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="H4:L25" xr:uid="{D0BB9C06-469C-46FE-BB4D-C953A54DDCD0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A29C7D30-099F-444F-9739-E051CD67CD3B}" name="Description" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{30C477D9-5C0B-4CDF-A3E5-B4A2E83DF121}" name="Binding" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2E0CFF8B-5D32-4B21-A1FD-ED03A30E5007}" name="Observable" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{82C1685A-B6EC-4953-9448-D9DB4262A589}" name="EnvironmentObject" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{58979CDD-4AAB-47D7-8792-46D7CDEAC059}" name="ObservableObject" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50FF2F7C-385A-4552-92CF-057D73BA5B98}" name="Tabel32" displayName="Tabel32" ref="B4:F25" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="B4:F25" xr:uid="{98762B35-F5B4-4A66-829F-8C9732910B18}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B4AED8B2-A0F7-4721-B110-917050B39E42}" name="Description" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{18B2743F-F921-4048-899E-B3A0C0D97122}" name="Binding" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{38CD2C64-8074-448B-BCB3-348D7E4A7AAE}" name="Observable" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{57256F41-676F-410A-83DC-964A697EF064}" name="EnvironmentObject" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{E6B185CC-255A-4BEB-AC7C-E59511F8AF6B}" name="ObservableObject" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3841660C-41A6-497A-AED2-9886A128CFA3}" name="Tabel326" displayName="Tabel326" ref="H4:L25" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="H4:L25" xr:uid="{3841660C-41A6-497A-AED2-9886A128CFA3}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{88ED316D-15D4-421B-9B57-9898B4E38658}" name="Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A0BF15F5-2379-4345-B15F-2853CFAA17AA}" name="Binding" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FC0CBF33-7BE3-4FED-A67E-B93470CAAA9F}" name="Observable" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3BC3DCEB-982A-43E3-B9DD-E106E08AE63A}" name="EnvironmentObject" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{73BFBF68-0096-4477-BEDE-B76BBB45872F}" name="ObservableObject" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C92186F-EC08-44BD-AD88-BB025BDCE7D7}" name="Tabel323" displayName="Tabel323" ref="B4:F25" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B4:F25" xr:uid="{98762B35-F5B4-4A66-829F-8C9732910B18}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0C983FBA-E5DA-4B32-9D96-56505CEDF67A}" name="Description" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{447D4271-3E59-4BC1-9E69-8B45ED9DF798}" name="Binding" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{9AEC545A-D4FC-4718-88A4-CBC2106BBCEF}" name="Observable" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{45BE3F2B-C5AD-49D2-9C6C-27FD456EA8CE}" name="EnvironmentObject" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{D116942C-C98A-4A58-B579-59B879D5C508}" name="ObservableObject" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,10 +1224,1409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD684293-54D6-4CBB-AE8F-4E16AED09FE4}">
-  <dimension ref="B4:F29"/>
+  <dimension ref="B4:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1">
+        <v>10</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>10</v>
+      </c>
+      <c r="L8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>10</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="6">
+        <v>20</v>
+      </c>
+      <c r="J9" s="5">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5">
+        <v>10</v>
+      </c>
+      <c r="L9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="1">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1">
+        <v>10</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="7">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7">
+        <v>20</v>
+      </c>
+      <c r="E22" s="5">
+        <v>10</v>
+      </c>
+      <c r="F22" s="5">
+        <v>10</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="7">
+        <v>20</v>
+      </c>
+      <c r="J22" s="7">
+        <v>20</v>
+      </c>
+      <c r="K22" s="5">
+        <v>10</v>
+      </c>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7E4E0A-3142-4B08-9187-4242C8A0012E}">
+  <dimension ref="B4:L29"/>
+  <sheetViews>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>99</v>
+      </c>
+      <c r="E7" s="1">
+        <v>90</v>
+      </c>
+      <c r="F7" s="1">
+        <v>90</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>90</v>
+      </c>
+      <c r="J7" s="1">
+        <v>99</v>
+      </c>
+      <c r="K7" s="1">
+        <v>90</v>
+      </c>
+      <c r="L7" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
+        <v>90</v>
+      </c>
+      <c r="F9" s="1">
+        <v>90</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="7">
+        <v>100</v>
+      </c>
+      <c r="J9" s="7">
+        <v>100</v>
+      </c>
+      <c r="K9" s="5">
+        <v>90</v>
+      </c>
+      <c r="L9" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1">
+        <v>90</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>90</v>
+      </c>
+      <c r="F20" s="1">
+        <v>90</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1">
+        <v>90</v>
+      </c>
+      <c r="J20" s="1">
+        <v>9</v>
+      </c>
+      <c r="K20" s="1">
+        <v>90</v>
+      </c>
+      <c r="L20" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>90</v>
+      </c>
+      <c r="F22" s="1">
+        <v>90</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="7">
+        <v>100</v>
+      </c>
+      <c r="J22" s="5">
+        <v>10</v>
+      </c>
+      <c r="K22" s="1">
+        <v>90</v>
+      </c>
+      <c r="L22" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0270B3-4E34-400C-895F-E08EB83E0B01}">
+  <dimension ref="B4:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +2669,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -732,50 +2686,50 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>10</v>
+        <v>4410</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
+        <v>4410</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>4410</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
+      <c r="C9" s="7">
+        <v>4420</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4410</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4410</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4410</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -792,7 +2746,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -809,16 +2763,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -826,33 +2780,33 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>47</v>
+      <c r="C14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -860,7 +2814,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -877,16 +2831,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -894,16 +2848,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -919,17 +2873,17 @@
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>17</v>
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -937,50 +2891,50 @@
         <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>10</v>
+        <v>4410</v>
       </c>
       <c r="D20" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>4410</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="1">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1">
-        <v>10</v>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="1">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1">
-        <v>20</v>
+      <c r="C22" s="7">
+        <v>4420</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>10</v>
+        <v>4410</v>
       </c>
       <c r="F22" s="1">
-        <v>10</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -996,49 +2950,60 @@
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>46</v>
+      <c r="C24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>49</v>
+      <c r="C25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="D27" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>28</v>
       </c>
+      <c r="D28" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>